<commit_message>
Add competitors to 30
</commit_message>
<xml_diff>
--- a/resources/data-csv/最美&最受歡迎女youtuber-整理版.xlsx
+++ b/resources/data-csv/最美&最受歡迎女youtuber-整理版.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenlich/Downloads/youtuber-pk/src/data-csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenlich/Downloads/youtuber-pk/resources/data-csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AFA77D-2CA9-9945-8B66-C071CA30220A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A1F3B-F4BD-2F4F-B89D-E73915D1B61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="最受歡迎" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="244">
   <si>
     <t>TheKellyYang</t>
   </si>
@@ -871,6 +871,84 @@
   </si>
   <si>
     <t>241182651_167679725439806_1419996355827098072_n</t>
+  </si>
+  <si>
+    <t>161436005_305726720975862_3227068468959228033_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCscRCnRkxjTfaJSqNOH7YBQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCyD3eaCai2yyWZEuczgZ-fw</t>
+  </si>
+  <si>
+    <t>231937424_189684746548630_7264873662462821473_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCbcFvHTFnj2cUiJXY6yUW9A</t>
+  </si>
+  <si>
+    <t>244711285_421984829529391_8074555302005882812_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/CindyH32</t>
+  </si>
+  <si>
+    <t>156216828_2825318357728242_1433282894302331460_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCjZCm3uuhkCvTYE9txucVcw</t>
+  </si>
+  <si>
+    <t>160242799_3746854308697543_3564161034818529210_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCAKJ0tmI_RMXqTgxL_OMfIg</t>
+  </si>
+  <si>
+    <t>253034702_1052538712236585_2442301185572619721_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/%E7%99%BD%E7%99%A1%E5%85%AC%E4%B8%BB</t>
+  </si>
+  <si>
+    <t>142934226_722980681925830_8961268986758795597_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/%E5%A3%B9%E5%8A%A0%E5%A3%B9</t>
+  </si>
+  <si>
+    <t>238767860_1392292497819165_7978461905279517538_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/blaire228</t>
+  </si>
+  <si>
+    <t>176125038_1737884546371643_4681262433306613349_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/NANACIAOCIAO</t>
+  </si>
+  <si>
+    <t>243366623_112603917843487_1885795655044618933_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UC2sk23-OLSaoT977mmVOPAw</t>
+  </si>
+  <si>
+    <t>129763366_144913980731427_7278780177754146576_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/AstorLiu</t>
+  </si>
+  <si>
+    <t>253852117_319775702869240_1608143372252872981_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCGpNjY0Xq2GJLXh4OOX1LOA</t>
+  </si>
+  <si>
+    <t>240453318_523924435363425_5985235544373995888_n</t>
   </si>
 </sst>
 </file>
@@ -7833,8 +7911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B925B9CE-F33D-7B44-856A-707AF1EDDBD7}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -8038,65 +8116,143 @@
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C20" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="B21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="B22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B23" t="s">
+        <v>229</v>
+      </c>
+      <c r="C23" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="B24" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="B25" t="s">
+        <v>233</v>
+      </c>
+      <c r="C25" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="B26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="B27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="B28" t="s">
+        <v>239</v>
+      </c>
+      <c r="C28" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="B29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>243</v>
+      </c>
+      <c r="C30" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:3">

</xml_diff>

<commit_message>
Add to 30 competitors
</commit_message>
<xml_diff>
--- a/resources/data-csv/最美&最受歡迎女youtuber-整理版.xlsx
+++ b/resources/data-csv/最美&最受歡迎女youtuber-整理版.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenlich/Downloads/youtuber-pk/resources/data-csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A1F3B-F4BD-2F4F-B89D-E73915D1B61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD153CE-229A-2F47-8084-563A5E8B4DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="246">
   <si>
     <t>TheKellyYang</t>
   </si>
@@ -949,6 +949,12 @@
   </si>
   <si>
     <t>240453318_523924435363425_5985235544373995888_n</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/JuliaLion%E5%92%AA%E5%A6%83%E5%A8%98%E5%A8%98</t>
+  </si>
+  <si>
+    <t>240315639_579186969927567_7881360356240474008_n</t>
   </si>
 </sst>
 </file>
@@ -7911,8 +7917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B925B9CE-F33D-7B44-856A-707AF1EDDBD7}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -8259,6 +8265,12 @@
       <c r="A31" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="B31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">

</xml_diff>